<commit_message>
Add test for minimum/maximum conditional formatting. Fix test for LowMidHigh (don't output values)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFColorScaleLowMidHigh.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFColorScaleLowMidHigh.xlsx
@@ -402,9 +402,9 @@
   <x:conditionalFormatting sqref="A1:A4">
     <x:cfRule type="colorScale" priority="1">
       <x:colorScale>
-        <x:cfvo type="min" val="0"/>
+        <x:cfvo type="min"/>
         <x:cfvo type="percent" val="50"/>
-        <x:cfvo type="max" val="0"/>
+        <x:cfvo type="max"/>
         <x:color rgb="FFFF0000"/>
         <x:color rgb="FFFFFF00"/>
         <x:color rgb="FF008000"/>

</xml_diff>